<commit_message>
Updates to Vanern rain values, parameter inputs
</commit_message>
<xml_diff>
--- a/VanernLake/ParameterInputsVanern.xlsx
+++ b/VanernLake/ParameterInputsVanern.xlsx
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,6 +555,9 @@
       <c r="A12" t="s">
         <v>14</v>
       </c>
+      <c r="B12">
+        <v>0.61470000000000002</v>
+      </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
@@ -563,6 +566,9 @@
       <c r="A13" t="s">
         <v>16</v>
       </c>
+      <c r="B13">
+        <v>3.6999999999999998E-2</v>
+      </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
@@ -571,6 +577,9 @@
       <c r="A14" t="s">
         <v>17</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
       <c r="C14" t="s">
         <v>30</v>
       </c>
@@ -579,6 +588,9 @@
       <c r="A15" t="s">
         <v>18</v>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
       <c r="C15" t="s">
         <v>31</v>
       </c>
@@ -587,6 +599,9 @@
       <c r="A16" t="s">
         <v>19</v>
       </c>
+      <c r="B16">
+        <v>0.2</v>
+      </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
@@ -595,6 +610,9 @@
       <c r="A17" t="s">
         <v>20</v>
       </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
@@ -603,6 +621,9 @@
       <c r="A18" t="s">
         <v>21</v>
       </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
       <c r="C18" t="s">
         <v>22</v>
       </c>
@@ -610,6 +631,9 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Update Vanern depth to mean depth
</commit_message>
<xml_diff>
--- a/VanernLake/ParameterInputsVanern.xlsx
+++ b/VanernLake/ParameterInputsVanern.xlsx
@@ -428,7 +428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -439,7 +439,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Vanern parameter update to test calibration. House keeping of old code.
</commit_message>
<xml_diff>
--- a/VanernLake/ParameterInputsVanern.xlsx
+++ b/VanernLake/ParameterInputsVanern.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\SOS\VanernLake\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="12195" yWindow="540" windowWidth="5175" windowHeight="7770"/>
   </bookViews>
@@ -428,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -438,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>0.01</v>
+        <v>1.0363000000000001E-2</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -649,7 +654,7 @@
         <v>29</v>
       </c>
       <c r="B21">
-        <v>3.0000000000000001E-3</v>
+        <v>3.3470000000000001E-3</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -660,7 +665,7 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>1E-3</v>
+        <v>1.4819E-3</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>

</xml_diff>